<commit_message>
Repo CUSTOMERS and ORDERS Working
</commit_message>
<xml_diff>
--- a/Output/Japan/Japan.xlsx
+++ b/Output/Japan/Japan.xlsx
@@ -6,17 +6,17 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="CUSTOMERS" r:id="rId8" sheetId="6"/>
-    <sheet name="ORDERS" r:id="rId9" sheetId="7"/>
-    <sheet name="PRODUCTS" r:id="rId10" sheetId="8"/>
-    <sheet name="DIM_TIME" r:id="rId11" sheetId="9"/>
-    <sheet name="FACT" r:id="rId7" sheetId="10"/>
+    <sheet name="CUSTOMERS" r:id="rId8" sheetId="11"/>
+    <sheet name="ORDERS" r:id="rId9" sheetId="12"/>
+    <sheet name="PRODUCTS" r:id="rId10" sheetId="13"/>
+    <sheet name="DIM_TIME" r:id="rId11" sheetId="14"/>
+    <sheet name="FACT" r:id="rId7" sheetId="15"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="182">
   <si>
     <t>CUSTOMERNUMBER</t>
   </si>
@@ -514,6 +514,54 @@
   </si>
   <si>
     <t>22/04/2005</t>
+  </si>
+  <si>
+    <t>2004/01/12</t>
+  </si>
+  <si>
+    <t>2004/01/22</t>
+  </si>
+  <si>
+    <t>2004/01/20</t>
+  </si>
+  <si>
+    <t>2004/04/13</t>
+  </si>
+  <si>
+    <t>2004/04/20</t>
+  </si>
+  <si>
+    <t>2004/06/15</t>
+  </si>
+  <si>
+    <t>2004/06/25</t>
+  </si>
+  <si>
+    <t>2004/06/23</t>
+  </si>
+  <si>
+    <t>2004/11/23</t>
+  </si>
+  <si>
+    <t>2004/11/30</t>
+  </si>
+  <si>
+    <t>2005/01/26</t>
+  </si>
+  <si>
+    <t>2005/02/05</t>
+  </si>
+  <si>
+    <t>2005/01/28</t>
+  </si>
+  <si>
+    <t>2005/04/22</t>
+  </si>
+  <si>
+    <t>2005/04/29</t>
+  </si>
+  <si>
+    <t>2005/04/27</t>
   </si>
 </sst>
 </file>
@@ -552,8 +600,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -564,1088 +615,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="false"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="19.48828125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="14.89453125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.65625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.203125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="10.39453125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="19.42578125" customWidth="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2300.0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>23.0</v>
-      </c>
-      <c r="F2" s="6" t="n">
-        <v>338433.27</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>3400.0</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="F3" s="6" t="n">
-        <v>500292.66000000003</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>3100.0</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="F4" s="6" t="n">
-        <v>456149.19</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>3844.0</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>565624.9956</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>1986.8</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>292347.48732</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>2658.96</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="F7" s="6" t="n">
-        <v>391252.40330400004</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>1851.0</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>272365.2099</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>2018.4</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="F9" s="6" t="n">
-        <v>296997.26616</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>2840.0</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>417891.516</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>3675.86</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>46.0</v>
-      </c>
-      <c r="F11" s="6" t="n">
-        <v>540884.0521140001</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>2307.24</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="F12" s="6" t="n">
-        <v>339498.599076</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>1763.86</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>43.0</v>
-      </c>
-      <c r="F13" s="6" t="n">
-        <v>259543.003314</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>1649.55</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="F14" s="6" t="n">
-        <v>242722.869795</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>2592.72</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="F15" s="6" t="n">
-        <v>381505.525128</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>2500.0</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="F16" s="6" t="n">
-        <v>367862.25</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>2678.4</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="F17" s="6" t="n">
-        <v>394112.90016</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>2953.86</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="F18" s="6" t="n">
-        <v>434645.434314</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>4100.0</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="F19" s="6" t="n">
-        <v>603294.0900000001</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>3700.0</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>37.0</v>
-      </c>
-      <c r="F20" s="6" t="n">
-        <v>544436.13</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="0" t="n">
-        <v>177.0</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>3700.0</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>37.0</v>
-      </c>
-      <c r="F21" s="6" t="n">
-        <v>544436.13</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>3200.0</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>32.0</v>
-      </c>
-      <c r="F22" s="6" t="n">
-        <v>470863.68000000005</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>4100.0</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="F23" s="6" t="n">
-        <v>603294.0900000001</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>4100.0</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="F24" s="6" t="n">
-        <v>603294.0900000001</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>1257.27</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="F25" s="6" t="n">
-        <v>185000.868423</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>1228.2</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="F26" s="6" t="n">
-        <v>180723.36618</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>3641.4</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="F27" s="6" t="n">
-        <v>535813.43886</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>2756.8</v>
-      </c>
-      <c r="E28" s="0" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="F28" s="6" t="n">
-        <v>405649.06032000005</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>2990.13</v>
-      </c>
-      <c r="E29" s="0" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="F29" s="6" t="n">
-        <v>439982.37983700004</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <v>2700.0</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="F30" s="6" t="n">
-        <v>397291.23000000004</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D31" s="0" t="n">
-        <v>1864.8</v>
-      </c>
-      <c r="E31" s="0" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="F31" s="6" t="n">
-        <v>274395.80952</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>2278.53</v>
-      </c>
-      <c r="E32" s="0" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="F32" s="6" t="n">
-        <v>335274.06899700005</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D33" s="0" t="n">
-        <v>1063.65</v>
-      </c>
-      <c r="E33" s="0" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="F33" s="6" t="n">
-        <v>156510.672885</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D34" s="0" t="n">
-        <v>5500.0</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <v>55.0</v>
-      </c>
-      <c r="F34" s="6" t="n">
-        <v>809296.9500000001</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D35" s="0" t="n">
-        <v>5500.0</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <v>55.0</v>
-      </c>
-      <c r="F35" s="6" t="n">
-        <v>809296.9500000001</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D36" s="0" t="n">
-        <v>2891.01</v>
-      </c>
-      <c r="E36" s="0" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="F36" s="6" t="n">
-        <v>425397.3773490001</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D37" s="0" t="n">
-        <v>2493.12</v>
-      </c>
-      <c r="E37" s="0" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="F37" s="6" t="n">
-        <v>366849.893088</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D38" s="0" t="n">
-        <v>4361.4</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="F38" s="6" t="n">
-        <v>641757.76686</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D39" s="0" t="n">
-        <v>2200.0</v>
-      </c>
-      <c r="E39" s="0" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="F39" s="6" t="n">
-        <v>323718.78</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D40" s="0" t="n">
-        <v>3918.75</v>
-      </c>
-      <c r="E40" s="0" t="n">
-        <v>55.0</v>
-      </c>
-      <c r="F40" s="6" t="n">
-        <v>576624.076875</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D41" s="0" t="n">
-        <v>3717.5</v>
-      </c>
-      <c r="E41" s="0" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="F41" s="6" t="n">
-        <v>547011.16575</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>2893.0</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="F42" s="6" t="n">
-        <v>425690.19570000004</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D43" s="0" t="n">
-        <v>2060.37</v>
-      </c>
-      <c r="E43" s="0" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="F43" s="6" t="n">
-        <v>303172.937613</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>4000.0</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="F44" s="6" t="n">
-        <v>588579.6</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D45" s="0" t="n">
-        <v>3400.0</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="F45" s="6" t="n">
-        <v>500292.66000000003</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D46" s="0" t="n">
-        <v>2800.0</v>
-      </c>
-      <c r="E46" s="0" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="F46" s="6" t="n">
-        <v>412005.72000000003</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D47" s="0" t="n">
-        <v>2117.75</v>
-      </c>
-      <c r="E47" s="0" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="F47" s="6" t="n">
-        <v>311616.111975</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D48" s="0" t="n">
-        <v>4800.0</v>
-      </c>
-      <c r="E48" s="0" t="n">
-        <v>48.0</v>
-      </c>
-      <c r="F48" s="6" t="n">
-        <v>706295.52</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D49" s="0" t="n">
-        <v>3562.49</v>
-      </c>
-      <c r="E49" s="0" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="F49" s="6" t="n">
-        <v>524202.234801</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D50" s="0" t="n">
-        <v>3700.0</v>
-      </c>
-      <c r="E50" s="0" t="n">
-        <v>37.0</v>
-      </c>
-      <c r="F50" s="6" t="n">
-        <v>544436.13</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D51" s="0" t="n">
-        <v>1405.92</v>
-      </c>
-      <c r="E51" s="0" t="n">
-        <v>24.0</v>
-      </c>
-      <c r="F51" s="6" t="n">
-        <v>206873.957808</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D52" s="0" t="n">
-        <v>4400.0</v>
-      </c>
-      <c r="E52" s="0" t="n">
-        <v>44.0</v>
-      </c>
-      <c r="F52" s="6" t="n">
-        <v>647437.56</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="0" t="n">
-        <v>398.0</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="D53" s="0" t="n">
-        <v>553.95</v>
-      </c>
-      <c r="E53" s="0" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="F53" s="6" t="n">
-        <v>81510.91735500001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1736,7 +706,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -1776,14 +746,14 @@
       <c r="A2" t="n">
         <v>10210.0</v>
       </c>
-      <c r="B2" t="n">
-        <v>37998.0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>38008.0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>38006.0</v>
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" t="s">
+        <v>168</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -1796,14 +766,14 @@
       <c r="A3" s="0" t="n">
         <v>10240.0</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>38090.0</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>38097.0</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>38097.0</v>
+      <c r="B3" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>170</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>22</v>
@@ -1816,14 +786,14 @@
       <c r="A4" s="0" t="n">
         <v>10258.0</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>38153.0</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>38163.0</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>38161.0</v>
+      <c r="B4" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>173</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>22</v>
@@ -1836,14 +806,14 @@
       <c r="A5" s="0" t="n">
         <v>10339.0</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>38314.0</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>38321.0</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>38321.0</v>
+      <c r="B5" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>175</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>22</v>
@@ -1856,14 +826,14 @@
       <c r="A6" s="0" t="n">
         <v>10372.0</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>38378.0</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>38388.0</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>38380.0</v>
+      <c r="B6" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>178</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>22</v>
@@ -1876,14 +846,14 @@
       <c r="A7" s="0" t="n">
         <v>10408.0</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>38464.0</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>38471.0</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>38469.0</v>
+      <c r="B7" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>181</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>22</v>
@@ -1897,7 +867,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H46"/>
   <sheetViews>
@@ -1960,10 +930,10 @@
       <c r="F2" t="n">
         <v>7305.0</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="7" t="n">
         <v>14567.3451</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="H2" s="8" t="n">
         <v>31489.0086</v>
       </c>
     </row>
@@ -1986,10 +956,10 @@
       <c r="F3" s="0" t="n">
         <v>6625.0</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="7" t="n">
         <v>10152.9981</v>
       </c>
-      <c r="H3" s="5" t="n">
+      <c r="H3" s="8" t="n">
         <v>17510.2431</v>
       </c>
     </row>
@@ -2012,10 +982,10 @@
       <c r="F4" s="0" t="n">
         <v>5582.0</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="7" t="n">
         <v>13390.1859</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="8" t="n">
         <v>28546.1106</v>
       </c>
     </row>
@@ -2038,10 +1008,10 @@
       <c r="F5" s="0" t="n">
         <v>1579.0</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="7" t="n">
         <v>11477.3022</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="8" t="n">
         <v>20158.851300000002</v>
       </c>
     </row>
@@ -2064,10 +1034,10 @@
       <c r="F6" s="0" t="n">
         <v>6906.0</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="7" t="n">
         <v>13095.8961</v>
       </c>
-      <c r="H6" s="5" t="n">
+      <c r="H6" s="8" t="n">
         <v>22218.8799</v>
       </c>
     </row>
@@ -2090,10 +1060,10 @@
       <c r="F7" s="0" t="n">
         <v>1049.0</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="7" t="n">
         <v>12213.0267</v>
       </c>
-      <c r="H7" s="5" t="n">
+      <c r="H7" s="8" t="n">
         <v>25456.0677</v>
       </c>
     </row>
@@ -2116,10 +1086,10 @@
       <c r="F8" s="0" t="n">
         <v>2613.0</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="7" t="n">
         <v>8534.4042</v>
       </c>
-      <c r="H8" s="5" t="n">
+      <c r="H8" s="8" t="n">
         <v>17215.9533</v>
       </c>
     </row>
@@ -2142,10 +1112,10 @@
       <c r="F9" s="0" t="n">
         <v>3975.0</v>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G9" s="7" t="n">
         <v>12360.171600000001</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="8" t="n">
         <v>20894.575800000002</v>
       </c>
     </row>
@@ -2168,10 +1138,10 @@
       <c r="F10" s="0" t="n">
         <v>5330.0</v>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="G10" s="7" t="n">
         <v>11330.1573</v>
       </c>
-      <c r="H10" s="5" t="n">
+      <c r="H10" s="8" t="n">
         <v>23248.894200000002</v>
       </c>
     </row>
@@ -2194,10 +1164,10 @@
       <c r="F11" s="0" t="n">
         <v>9772.0</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="7" t="n">
         <v>13831.6206</v>
       </c>
-      <c r="H11" s="5" t="n">
+      <c r="H11" s="8" t="n">
         <v>20894.575800000002</v>
       </c>
     </row>
@@ -2220,10 +1190,10 @@
       <c r="F12" s="0" t="n">
         <v>992.0</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G12" s="7" t="n">
         <v>7210.100100000001</v>
       </c>
-      <c r="H12" s="5" t="n">
+      <c r="H12" s="8" t="n">
         <v>12360.171600000001</v>
       </c>
     </row>
@@ -2246,10 +1216,10 @@
       <c r="F13" s="0" t="n">
         <v>4357.0</v>
       </c>
-      <c r="G13" s="4" t="n">
+      <c r="G13" s="7" t="n">
         <v>3531.4776</v>
       </c>
-      <c r="H13" s="5" t="n">
+      <c r="H13" s="8" t="n">
         <v>8975.8389</v>
       </c>
     </row>
@@ -2272,10 +1242,10 @@
       <c r="F14" s="0" t="n">
         <v>3913.0</v>
       </c>
-      <c r="G14" s="4" t="n">
+      <c r="G14" s="7" t="n">
         <v>10005.853200000001</v>
       </c>
-      <c r="H14" s="5" t="n">
+      <c r="H14" s="8" t="n">
         <v>20158.851300000002</v>
       </c>
     </row>
@@ -2298,10 +1268,10 @@
       <c r="F15" s="0" t="n">
         <v>6450.0</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="7" t="n">
         <v>10005.853200000001</v>
       </c>
-      <c r="H15" s="5" t="n">
+      <c r="H15" s="8" t="n">
         <v>14861.634900000001</v>
       </c>
     </row>
@@ -2324,10 +1294,10 @@
       <c r="F16" s="0" t="n">
         <v>8990.0</v>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G16" s="7" t="n">
         <v>9122.9838</v>
       </c>
-      <c r="H16" s="5" t="n">
+      <c r="H16" s="8" t="n">
         <v>20747.4309</v>
       </c>
     </row>
@@ -2350,10 +1320,10 @@
       <c r="F17" s="0" t="n">
         <v>5545.0</v>
       </c>
-      <c r="G17" s="4" t="n">
+      <c r="G17" s="7" t="n">
         <v>13537.3308</v>
       </c>
-      <c r="H17" s="5" t="n">
+      <c r="H17" s="8" t="n">
         <v>21188.8656</v>
       </c>
     </row>
@@ -2376,10 +1346,10 @@
       <c r="F18" s="0" t="n">
         <v>8290.0</v>
       </c>
-      <c r="G18" s="4" t="n">
+      <c r="G18" s="7" t="n">
         <v>7798.679700000001</v>
       </c>
-      <c r="H18" s="5" t="n">
+      <c r="H18" s="8" t="n">
         <v>12948.7512</v>
       </c>
     </row>
@@ -2402,10 +1372,10 @@
       <c r="F19" s="0" t="n">
         <v>6645.0</v>
       </c>
-      <c r="G19" s="4" t="n">
+      <c r="G19" s="7" t="n">
         <v>3384.3327</v>
       </c>
-      <c r="H19" s="5" t="n">
+      <c r="H19" s="8" t="n">
         <v>7357.245000000001</v>
       </c>
     </row>
@@ -2428,10 +1398,10 @@
       <c r="F20" s="0" t="n">
         <v>7003.0</v>
       </c>
-      <c r="G20" s="4" t="n">
+      <c r="G20" s="7" t="n">
         <v>8975.8389</v>
       </c>
-      <c r="H20" s="5" t="n">
+      <c r="H20" s="8" t="n">
         <v>16627.3737</v>
       </c>
     </row>
@@ -2454,10 +1424,10 @@
       <c r="F21" s="0" t="n">
         <v>3627.0</v>
       </c>
-      <c r="G21" s="4" t="n">
+      <c r="G21" s="7" t="n">
         <v>9858.7083</v>
       </c>
-      <c r="H21" s="5" t="n">
+      <c r="H21" s="8" t="n">
         <v>16038.794100000001</v>
       </c>
     </row>
@@ -2480,10 +1450,10 @@
       <c r="F22" s="0" t="n">
         <v>15.0</v>
       </c>
-      <c r="G22" s="4" t="n">
+      <c r="G22" s="7" t="n">
         <v>5444.3613000000005</v>
       </c>
-      <c r="H22" s="5" t="n">
+      <c r="H22" s="8" t="n">
         <v>11183.0124</v>
       </c>
     </row>
@@ -2506,10 +1476,10 @@
       <c r="F23" s="0" t="n">
         <v>1898.0</v>
       </c>
-      <c r="G23" s="4" t="n">
+      <c r="G23" s="7" t="n">
         <v>12065.881800000001</v>
       </c>
-      <c r="H23" s="5" t="n">
+      <c r="H23" s="8" t="n">
         <v>18098.8227</v>
       </c>
     </row>
@@ -2532,10 +1502,10 @@
       <c r="F24" s="0" t="n">
         <v>5942.0</v>
       </c>
-      <c r="G24" s="4" t="n">
+      <c r="G24" s="7" t="n">
         <v>5002.926600000001</v>
       </c>
-      <c r="H24" s="5" t="n">
+      <c r="H24" s="8" t="n">
         <v>10152.9981</v>
       </c>
     </row>
@@ -2558,10 +1528,10 @@
       <c r="F25" s="0" t="n">
         <v>9173.0</v>
       </c>
-      <c r="G25" s="4" t="n">
+      <c r="G25" s="7" t="n">
         <v>6915.8103</v>
       </c>
-      <c r="H25" s="5" t="n">
+      <c r="H25" s="8" t="n">
         <v>13095.8961</v>
       </c>
     </row>
@@ -2584,10 +1554,10 @@
       <c r="F26" s="0" t="n">
         <v>2902.0</v>
       </c>
-      <c r="G26" s="4" t="n">
+      <c r="G26" s="7" t="n">
         <v>3825.7674</v>
       </c>
-      <c r="H26" s="5" t="n">
+      <c r="H26" s="8" t="n">
         <v>9711.563400000001</v>
       </c>
     </row>
@@ -2610,10 +1580,10 @@
       <c r="F27" s="0" t="n">
         <v>6621.0</v>
       </c>
-      <c r="G27" s="4" t="n">
+      <c r="G27" s="7" t="n">
         <v>7210.100100000001</v>
       </c>
-      <c r="H27" s="5" t="n">
+      <c r="H27" s="8" t="n">
         <v>12360.171600000001</v>
       </c>
     </row>
@@ -2636,10 +1606,10 @@
       <c r="F28" s="0" t="n">
         <v>6812.0</v>
       </c>
-      <c r="G28" s="4" t="n">
+      <c r="G28" s="7" t="n">
         <v>4267.2021</v>
       </c>
-      <c r="H28" s="5" t="n">
+      <c r="H28" s="8" t="n">
         <v>10005.853200000001</v>
       </c>
     </row>
@@ -2662,10 +1632,10 @@
       <c r="F29" s="0" t="n">
         <v>2081.0</v>
       </c>
-      <c r="G29" s="4" t="n">
+      <c r="G29" s="7" t="n">
         <v>3237.1878</v>
       </c>
-      <c r="H29" s="5" t="n">
+      <c r="H29" s="8" t="n">
         <v>6032.9409000000005</v>
       </c>
     </row>
@@ -2688,10 +1658,10 @@
       <c r="F30" s="0" t="n">
         <v>2756.0</v>
       </c>
-      <c r="G30" s="4" t="n">
+      <c r="G30" s="7" t="n">
         <v>5297.2164</v>
       </c>
-      <c r="H30" s="5" t="n">
+      <c r="H30" s="8" t="n">
         <v>10594.4328</v>
       </c>
     </row>
@@ -2714,10 +1684,10 @@
       <c r="F31" s="0" t="n">
         <v>178.0</v>
       </c>
-      <c r="G31" s="4" t="n">
+      <c r="G31" s="7" t="n">
         <v>9858.7083</v>
       </c>
-      <c r="H31" s="5" t="n">
+      <c r="H31" s="8" t="n">
         <v>14714.490000000002</v>
       </c>
     </row>
@@ -2740,10 +1710,10 @@
       <c r="F32" s="0" t="n">
         <v>814.0</v>
       </c>
-      <c r="G32" s="4" t="n">
+      <c r="G32" s="7" t="n">
         <v>5002.926600000001</v>
       </c>
-      <c r="H32" s="5" t="n">
+      <c r="H32" s="8" t="n">
         <v>9564.4185</v>
       </c>
     </row>
@@ -2766,10 +1736,10 @@
       <c r="F33" s="0" t="n">
         <v>136.0</v>
       </c>
-      <c r="G33" s="4" t="n">
+      <c r="G33" s="7" t="n">
         <v>4855.7817000000005</v>
       </c>
-      <c r="H33" s="5" t="n">
+      <c r="H33" s="8" t="n">
         <v>10152.9981</v>
       </c>
     </row>
@@ -2792,10 +1762,10 @@
       <c r="F34" s="0" t="n">
         <v>7062.0</v>
       </c>
-      <c r="G34" s="4" t="n">
+      <c r="G34" s="7" t="n">
         <v>3972.9123</v>
       </c>
-      <c r="H34" s="5" t="n">
+      <c r="H34" s="8" t="n">
         <v>6474.3756</v>
       </c>
     </row>
@@ -2818,10 +1788,10 @@
       <c r="F35" s="0" t="n">
         <v>1645.0</v>
       </c>
-      <c r="G35" s="4" t="n">
+      <c r="G35" s="7" t="n">
         <v>5444.3613000000005</v>
       </c>
-      <c r="H35" s="5" t="n">
+      <c r="H35" s="8" t="n">
         <v>8681.5491</v>
       </c>
     </row>
@@ -2844,10 +1814,10 @@
       <c r="F36" s="0" t="n">
         <v>1897.0</v>
       </c>
-      <c r="G36" s="4" t="n">
+      <c r="G36" s="7" t="n">
         <v>5002.926600000001</v>
       </c>
-      <c r="H36" s="5" t="n">
+      <c r="H36" s="8" t="n">
         <v>9858.7083</v>
       </c>
     </row>
@@ -2870,10 +1840,10 @@
       <c r="F37" s="0" t="n">
         <v>5841.0</v>
       </c>
-      <c r="G37" s="4" t="n">
+      <c r="G37" s="7" t="n">
         <v>7504.3899</v>
       </c>
-      <c r="H37" s="5" t="n">
+      <c r="H37" s="8" t="n">
         <v>13390.1859</v>
       </c>
     </row>
@@ -2896,10 +1866,10 @@
       <c r="F38" s="0" t="n">
         <v>737.0</v>
       </c>
-      <c r="G38" s="4" t="n">
+      <c r="G38" s="7" t="n">
         <v>6327.2307</v>
       </c>
-      <c r="H38" s="5" t="n">
+      <c r="H38" s="8" t="n">
         <v>12801.606300000001</v>
       </c>
     </row>
@@ -2922,10 +1892,10 @@
       <c r="F39" s="0" t="n">
         <v>3501.0</v>
       </c>
-      <c r="G39" s="4" t="n">
+      <c r="G39" s="7" t="n">
         <v>5885.796</v>
       </c>
-      <c r="H39" s="5" t="n">
+      <c r="H39" s="8" t="n">
         <v>13390.1859</v>
       </c>
     </row>
@@ -2948,10 +1918,10 @@
       <c r="F40" s="0" t="n">
         <v>9653.0</v>
       </c>
-      <c r="G40" s="4" t="n">
+      <c r="G40" s="7" t="n">
         <v>10152.9981</v>
       </c>
-      <c r="H40" s="5" t="n">
+      <c r="H40" s="8" t="n">
         <v>14714.490000000002</v>
       </c>
     </row>
@@ -2974,10 +1944,10 @@
       <c r="F41" s="0" t="n">
         <v>7083.0</v>
       </c>
-      <c r="G41" s="4" t="n">
+      <c r="G41" s="7" t="n">
         <v>5002.926600000001</v>
       </c>
-      <c r="H41" s="5" t="n">
+      <c r="H41" s="8" t="n">
         <v>10594.4328</v>
       </c>
     </row>
@@ -3000,10 +1970,10 @@
       <c r="F42" s="0" t="n">
         <v>6934.0</v>
       </c>
-      <c r="G42" s="4" t="n">
+      <c r="G42" s="7" t="n">
         <v>6915.8103</v>
       </c>
-      <c r="H42" s="5" t="n">
+      <c r="H42" s="8" t="n">
         <v>14861.634900000001</v>
       </c>
     </row>
@@ -3026,10 +1996,10 @@
       <c r="F43" s="0" t="n">
         <v>7106.0</v>
       </c>
-      <c r="G43" s="4" t="n">
+      <c r="G43" s="7" t="n">
         <v>8681.5491</v>
       </c>
-      <c r="H43" s="5" t="n">
+      <c r="H43" s="8" t="n">
         <v>17510.2431</v>
       </c>
     </row>
@@ -3052,10 +2022,10 @@
       <c r="F44" s="0" t="n">
         <v>551.0</v>
       </c>
-      <c r="G44" s="4" t="n">
+      <c r="G44" s="7" t="n">
         <v>7945.8246</v>
       </c>
-      <c r="H44" s="5" t="n">
+      <c r="H44" s="8" t="n">
         <v>11771.592</v>
       </c>
     </row>
@@ -3078,10 +2048,10 @@
       <c r="F45" s="0" t="n">
         <v>8820.0</v>
       </c>
-      <c r="G45" s="4" t="n">
+      <c r="G45" s="7" t="n">
         <v>5297.2164</v>
       </c>
-      <c r="H45" s="5" t="n">
+      <c r="H45" s="8" t="n">
         <v>10888.722600000001</v>
       </c>
     </row>
@@ -3104,10 +2074,10 @@
       <c r="F46" s="0" t="n">
         <v>4857.0</v>
       </c>
-      <c r="G46" s="4" t="n">
+      <c r="G46" s="7" t="n">
         <v>4855.7817000000005</v>
       </c>
-      <c r="H46" s="5" t="n">
+      <c r="H46" s="8" t="n">
         <v>7357.245000000001</v>
       </c>
     </row>
@@ -3116,7 +2086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -3137,7 +2107,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B2" t="n">
         <v>1.0</v>
@@ -3148,7 +2118,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B3" t="n">
         <v>4.0</v>
@@ -3159,7 +2129,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B4" t="n">
         <v>6.0</v>
@@ -3170,7 +2140,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B5" t="n">
         <v>11.0</v>
@@ -3181,7 +2151,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B6" t="n">
         <v>1.0</v>
@@ -3192,13 +2162,1094 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B7" t="n">
         <v>4.0</v>
       </c>
       <c r="C7" t="n">
         <v>2005.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:F53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="19.48828125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="14.89453125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.3046875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.203125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="10.39453125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="19.42578125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2300.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="F2" s="9" t="n">
+        <v>338433.27</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>3400.0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="F3" s="9" t="n">
+        <v>500292.66000000003</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3100.0</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="F4" s="9" t="n">
+        <v>456149.19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>3844.0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="F5" s="9" t="n">
+        <v>565624.9956</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1986.8</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="F6" s="9" t="n">
+        <v>292347.48732</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2658.96</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="F7" s="9" t="n">
+        <v>391252.40330400004</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1851.0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="F8" s="9" t="n">
+        <v>272365.2099</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>2018.4</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="F9" s="9" t="n">
+        <v>296997.26616</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>2840.0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="F10" s="9" t="n">
+        <v>417891.516</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>3675.86</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="F11" s="9" t="n">
+        <v>540884.0521140001</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>2307.24</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="F12" s="9" t="n">
+        <v>339498.599076</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1763.86</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="F13" s="9" t="n">
+        <v>259543.003314</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1649.55</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="F14" s="9" t="n">
+        <v>242722.869795</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>2592.72</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="F15" s="9" t="n">
+        <v>381505.525128</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>2500.0</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="F16" s="9" t="n">
+        <v>367862.25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>2678.4</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="F17" s="9" t="n">
+        <v>394112.90016</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>2953.86</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="F18" s="9" t="n">
+        <v>434645.434314</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>4100.0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="F19" s="9" t="n">
+        <v>603294.0900000001</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>3700.0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="F20" s="9" t="n">
+        <v>544436.13</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>3700.0</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="F21" s="9" t="n">
+        <v>544436.13</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>3200.0</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="F22" s="9" t="n">
+        <v>470863.68000000005</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>4100.0</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="F23" s="9" t="n">
+        <v>603294.0900000001</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>4100.0</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="F24" s="9" t="n">
+        <v>603294.0900000001</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>1257.27</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="F25" s="9" t="n">
+        <v>185000.868423</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>1228.2</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="F26" s="9" t="n">
+        <v>180723.36618</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>3641.4</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="F27" s="9" t="n">
+        <v>535813.43886</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>2756.8</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="F28" s="9" t="n">
+        <v>405649.06032000005</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>2990.13</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="F29" s="9" t="n">
+        <v>439982.37983700004</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>2700.0</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="F30" s="9" t="n">
+        <v>397291.23000000004</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>1864.8</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="F31" s="9" t="n">
+        <v>274395.80952</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>2278.53</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="F32" s="9" t="n">
+        <v>335274.06899700005</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>1063.65</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="F33" s="9" t="n">
+        <v>156510.672885</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>5500.0</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="F34" s="9" t="n">
+        <v>809296.9500000001</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>5500.0</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="F35" s="9" t="n">
+        <v>809296.9500000001</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>2891.01</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="F36" s="9" t="n">
+        <v>425397.3773490001</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>2493.12</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="F37" s="9" t="n">
+        <v>366849.893088</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>4361.4</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="F38" s="9" t="n">
+        <v>641757.76686</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>2200.0</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="F39" s="9" t="n">
+        <v>323718.78</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>3918.75</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="F40" s="9" t="n">
+        <v>576624.076875</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>3717.5</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="F41" s="9" t="n">
+        <v>547011.16575</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>2893.0</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="F42" s="9" t="n">
+        <v>425690.19570000004</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>2060.37</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="F43" s="9" t="n">
+        <v>303172.937613</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>4000.0</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="F44" s="9" t="n">
+        <v>588579.6</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>3400.0</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="F45" s="9" t="n">
+        <v>500292.66000000003</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>2800.0</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="F46" s="9" t="n">
+        <v>412005.72000000003</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>2117.75</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="F47" s="9" t="n">
+        <v>311616.111975</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>4800.0</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="F48" s="9" t="n">
+        <v>706295.52</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>3562.49</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="F49" s="9" t="n">
+        <v>524202.234801</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>3700.0</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="F50" s="9" t="n">
+        <v>544436.13</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>1405.92</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="F51" s="9" t="n">
+        <v>206873.957808</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>4400.0</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="F52" s="9" t="n">
+        <v>647437.56</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="n">
+        <v>398.0</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>553.95</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="F53" s="9" t="n">
+        <v>81510.91735500001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Repository with Japan, France (Sales bugged) and Singapore
</commit_message>
<xml_diff>
--- a/Output/Japan/Japan.xlsx
+++ b/Output/Japan/Japan.xlsx
@@ -6,17 +6,17 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="CUSTOMERS" r:id="rId8" sheetId="41"/>
-    <sheet name="ORDERS" r:id="rId9" sheetId="42"/>
-    <sheet name="PRODUCTS" r:id="rId10" sheetId="43"/>
-    <sheet name="DIM_TIME" r:id="rId11" sheetId="44"/>
-    <sheet name="FACT" r:id="rId7" sheetId="45"/>
+    <sheet name="CUSTOMERS" r:id="rId8" sheetId="71"/>
+    <sheet name="ORDERS" r:id="rId9" sheetId="72"/>
+    <sheet name="PRODUCTS" r:id="rId10" sheetId="73"/>
+    <sheet name="DIM_TIME" r:id="rId11" sheetId="74"/>
+    <sheet name="FACT" r:id="rId7" sheetId="75"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3506" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5916" uniqueCount="182">
   <si>
     <t>CUSTOMERNUMBER</t>
   </si>
@@ -600,8 +600,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -633,7 +651,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -724,7 +742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -885,7 +903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H46"/>
   <sheetViews>
@@ -948,10 +966,10 @@
       <c r="F2" t="n">
         <v>7305.0</v>
       </c>
-      <c r="G2" s="25" t="n">
+      <c r="G2" s="43" t="n">
         <v>14567.3451</v>
       </c>
-      <c r="H2" s="26" t="n">
+      <c r="H2" s="44" t="n">
         <v>31489.0086</v>
       </c>
     </row>
@@ -974,10 +992,10 @@
       <c r="F3" s="0" t="n">
         <v>6625.0</v>
       </c>
-      <c r="G3" s="25" t="n">
+      <c r="G3" s="43" t="n">
         <v>10152.9981</v>
       </c>
-      <c r="H3" s="26" t="n">
+      <c r="H3" s="44" t="n">
         <v>17510.2431</v>
       </c>
     </row>
@@ -1000,10 +1018,10 @@
       <c r="F4" s="0" t="n">
         <v>5582.0</v>
       </c>
-      <c r="G4" s="25" t="n">
+      <c r="G4" s="43" t="n">
         <v>13390.1859</v>
       </c>
-      <c r="H4" s="26" t="n">
+      <c r="H4" s="44" t="n">
         <v>28546.1106</v>
       </c>
     </row>
@@ -1026,10 +1044,10 @@
       <c r="F5" s="0" t="n">
         <v>1579.0</v>
       </c>
-      <c r="G5" s="25" t="n">
+      <c r="G5" s="43" t="n">
         <v>11477.3022</v>
       </c>
-      <c r="H5" s="26" t="n">
+      <c r="H5" s="44" t="n">
         <v>20158.851300000002</v>
       </c>
     </row>
@@ -1052,10 +1070,10 @@
       <c r="F6" s="0" t="n">
         <v>6906.0</v>
       </c>
-      <c r="G6" s="25" t="n">
+      <c r="G6" s="43" t="n">
         <v>13095.8961</v>
       </c>
-      <c r="H6" s="26" t="n">
+      <c r="H6" s="44" t="n">
         <v>22218.8799</v>
       </c>
     </row>
@@ -1078,10 +1096,10 @@
       <c r="F7" s="0" t="n">
         <v>1049.0</v>
       </c>
-      <c r="G7" s="25" t="n">
+      <c r="G7" s="43" t="n">
         <v>12213.0267</v>
       </c>
-      <c r="H7" s="26" t="n">
+      <c r="H7" s="44" t="n">
         <v>25456.0677</v>
       </c>
     </row>
@@ -1104,10 +1122,10 @@
       <c r="F8" s="0" t="n">
         <v>2613.0</v>
       </c>
-      <c r="G8" s="25" t="n">
+      <c r="G8" s="43" t="n">
         <v>8534.4042</v>
       </c>
-      <c r="H8" s="26" t="n">
+      <c r="H8" s="44" t="n">
         <v>17215.9533</v>
       </c>
     </row>
@@ -1130,10 +1148,10 @@
       <c r="F9" s="0" t="n">
         <v>3975.0</v>
       </c>
-      <c r="G9" s="25" t="n">
+      <c r="G9" s="43" t="n">
         <v>12360.171600000001</v>
       </c>
-      <c r="H9" s="26" t="n">
+      <c r="H9" s="44" t="n">
         <v>20894.575800000002</v>
       </c>
     </row>
@@ -1156,10 +1174,10 @@
       <c r="F10" s="0" t="n">
         <v>5330.0</v>
       </c>
-      <c r="G10" s="25" t="n">
+      <c r="G10" s="43" t="n">
         <v>11330.1573</v>
       </c>
-      <c r="H10" s="26" t="n">
+      <c r="H10" s="44" t="n">
         <v>23248.894200000002</v>
       </c>
     </row>
@@ -1182,10 +1200,10 @@
       <c r="F11" s="0" t="n">
         <v>9772.0</v>
       </c>
-      <c r="G11" s="25" t="n">
+      <c r="G11" s="43" t="n">
         <v>13831.6206</v>
       </c>
-      <c r="H11" s="26" t="n">
+      <c r="H11" s="44" t="n">
         <v>20894.575800000002</v>
       </c>
     </row>
@@ -1208,10 +1226,10 @@
       <c r="F12" s="0" t="n">
         <v>992.0</v>
       </c>
-      <c r="G12" s="25" t="n">
+      <c r="G12" s="43" t="n">
         <v>7210.100100000001</v>
       </c>
-      <c r="H12" s="26" t="n">
+      <c r="H12" s="44" t="n">
         <v>12360.171600000001</v>
       </c>
     </row>
@@ -1234,10 +1252,10 @@
       <c r="F13" s="0" t="n">
         <v>4357.0</v>
       </c>
-      <c r="G13" s="25" t="n">
+      <c r="G13" s="43" t="n">
         <v>3531.4776</v>
       </c>
-      <c r="H13" s="26" t="n">
+      <c r="H13" s="44" t="n">
         <v>8975.8389</v>
       </c>
     </row>
@@ -1260,10 +1278,10 @@
       <c r="F14" s="0" t="n">
         <v>3913.0</v>
       </c>
-      <c r="G14" s="25" t="n">
+      <c r="G14" s="43" t="n">
         <v>10005.853200000001</v>
       </c>
-      <c r="H14" s="26" t="n">
+      <c r="H14" s="44" t="n">
         <v>20158.851300000002</v>
       </c>
     </row>
@@ -1286,10 +1304,10 @@
       <c r="F15" s="0" t="n">
         <v>6450.0</v>
       </c>
-      <c r="G15" s="25" t="n">
+      <c r="G15" s="43" t="n">
         <v>10005.853200000001</v>
       </c>
-      <c r="H15" s="26" t="n">
+      <c r="H15" s="44" t="n">
         <v>14861.634900000001</v>
       </c>
     </row>
@@ -1312,10 +1330,10 @@
       <c r="F16" s="0" t="n">
         <v>8990.0</v>
       </c>
-      <c r="G16" s="25" t="n">
+      <c r="G16" s="43" t="n">
         <v>9122.9838</v>
       </c>
-      <c r="H16" s="26" t="n">
+      <c r="H16" s="44" t="n">
         <v>20747.4309</v>
       </c>
     </row>
@@ -1338,10 +1356,10 @@
       <c r="F17" s="0" t="n">
         <v>5545.0</v>
       </c>
-      <c r="G17" s="25" t="n">
+      <c r="G17" s="43" t="n">
         <v>13537.3308</v>
       </c>
-      <c r="H17" s="26" t="n">
+      <c r="H17" s="44" t="n">
         <v>21188.8656</v>
       </c>
     </row>
@@ -1364,10 +1382,10 @@
       <c r="F18" s="0" t="n">
         <v>8290.0</v>
       </c>
-      <c r="G18" s="25" t="n">
+      <c r="G18" s="43" t="n">
         <v>7798.679700000001</v>
       </c>
-      <c r="H18" s="26" t="n">
+      <c r="H18" s="44" t="n">
         <v>12948.7512</v>
       </c>
     </row>
@@ -1390,10 +1408,10 @@
       <c r="F19" s="0" t="n">
         <v>6645.0</v>
       </c>
-      <c r="G19" s="25" t="n">
+      <c r="G19" s="43" t="n">
         <v>3384.3327</v>
       </c>
-      <c r="H19" s="26" t="n">
+      <c r="H19" s="44" t="n">
         <v>7357.245000000001</v>
       </c>
     </row>
@@ -1416,10 +1434,10 @@
       <c r="F20" s="0" t="n">
         <v>7003.0</v>
       </c>
-      <c r="G20" s="25" t="n">
+      <c r="G20" s="43" t="n">
         <v>8975.8389</v>
       </c>
-      <c r="H20" s="26" t="n">
+      <c r="H20" s="44" t="n">
         <v>16627.3737</v>
       </c>
     </row>
@@ -1442,10 +1460,10 @@
       <c r="F21" s="0" t="n">
         <v>3627.0</v>
       </c>
-      <c r="G21" s="25" t="n">
+      <c r="G21" s="43" t="n">
         <v>9858.7083</v>
       </c>
-      <c r="H21" s="26" t="n">
+      <c r="H21" s="44" t="n">
         <v>16038.794100000001</v>
       </c>
     </row>
@@ -1468,10 +1486,10 @@
       <c r="F22" s="0" t="n">
         <v>15.0</v>
       </c>
-      <c r="G22" s="25" t="n">
+      <c r="G22" s="43" t="n">
         <v>5444.3613000000005</v>
       </c>
-      <c r="H22" s="26" t="n">
+      <c r="H22" s="44" t="n">
         <v>11183.0124</v>
       </c>
     </row>
@@ -1494,10 +1512,10 @@
       <c r="F23" s="0" t="n">
         <v>1898.0</v>
       </c>
-      <c r="G23" s="25" t="n">
+      <c r="G23" s="43" t="n">
         <v>12065.881800000001</v>
       </c>
-      <c r="H23" s="26" t="n">
+      <c r="H23" s="44" t="n">
         <v>18098.8227</v>
       </c>
     </row>
@@ -1520,10 +1538,10 @@
       <c r="F24" s="0" t="n">
         <v>5942.0</v>
       </c>
-      <c r="G24" s="25" t="n">
+      <c r="G24" s="43" t="n">
         <v>5002.926600000001</v>
       </c>
-      <c r="H24" s="26" t="n">
+      <c r="H24" s="44" t="n">
         <v>10152.9981</v>
       </c>
     </row>
@@ -1546,10 +1564,10 @@
       <c r="F25" s="0" t="n">
         <v>9173.0</v>
       </c>
-      <c r="G25" s="25" t="n">
+      <c r="G25" s="43" t="n">
         <v>6915.8103</v>
       </c>
-      <c r="H25" s="26" t="n">
+      <c r="H25" s="44" t="n">
         <v>13095.8961</v>
       </c>
     </row>
@@ -1572,10 +1590,10 @@
       <c r="F26" s="0" t="n">
         <v>2902.0</v>
       </c>
-      <c r="G26" s="25" t="n">
+      <c r="G26" s="43" t="n">
         <v>3825.7674</v>
       </c>
-      <c r="H26" s="26" t="n">
+      <c r="H26" s="44" t="n">
         <v>9711.563400000001</v>
       </c>
     </row>
@@ -1598,10 +1616,10 @@
       <c r="F27" s="0" t="n">
         <v>6621.0</v>
       </c>
-      <c r="G27" s="25" t="n">
+      <c r="G27" s="43" t="n">
         <v>7210.100100000001</v>
       </c>
-      <c r="H27" s="26" t="n">
+      <c r="H27" s="44" t="n">
         <v>12360.171600000001</v>
       </c>
     </row>
@@ -1624,10 +1642,10 @@
       <c r="F28" s="0" t="n">
         <v>6812.0</v>
       </c>
-      <c r="G28" s="25" t="n">
+      <c r="G28" s="43" t="n">
         <v>4267.2021</v>
       </c>
-      <c r="H28" s="26" t="n">
+      <c r="H28" s="44" t="n">
         <v>10005.853200000001</v>
       </c>
     </row>
@@ -1650,10 +1668,10 @@
       <c r="F29" s="0" t="n">
         <v>2081.0</v>
       </c>
-      <c r="G29" s="25" t="n">
+      <c r="G29" s="43" t="n">
         <v>3237.1878</v>
       </c>
-      <c r="H29" s="26" t="n">
+      <c r="H29" s="44" t="n">
         <v>6032.9409000000005</v>
       </c>
     </row>
@@ -1676,10 +1694,10 @@
       <c r="F30" s="0" t="n">
         <v>2756.0</v>
       </c>
-      <c r="G30" s="25" t="n">
+      <c r="G30" s="43" t="n">
         <v>5297.2164</v>
       </c>
-      <c r="H30" s="26" t="n">
+      <c r="H30" s="44" t="n">
         <v>10594.4328</v>
       </c>
     </row>
@@ -1702,10 +1720,10 @@
       <c r="F31" s="0" t="n">
         <v>178.0</v>
       </c>
-      <c r="G31" s="25" t="n">
+      <c r="G31" s="43" t="n">
         <v>9858.7083</v>
       </c>
-      <c r="H31" s="26" t="n">
+      <c r="H31" s="44" t="n">
         <v>14714.490000000002</v>
       </c>
     </row>
@@ -1728,10 +1746,10 @@
       <c r="F32" s="0" t="n">
         <v>814.0</v>
       </c>
-      <c r="G32" s="25" t="n">
+      <c r="G32" s="43" t="n">
         <v>5002.926600000001</v>
       </c>
-      <c r="H32" s="26" t="n">
+      <c r="H32" s="44" t="n">
         <v>9564.4185</v>
       </c>
     </row>
@@ -1754,10 +1772,10 @@
       <c r="F33" s="0" t="n">
         <v>136.0</v>
       </c>
-      <c r="G33" s="25" t="n">
+      <c r="G33" s="43" t="n">
         <v>4855.7817000000005</v>
       </c>
-      <c r="H33" s="26" t="n">
+      <c r="H33" s="44" t="n">
         <v>10152.9981</v>
       </c>
     </row>
@@ -1780,10 +1798,10 @@
       <c r="F34" s="0" t="n">
         <v>7062.0</v>
       </c>
-      <c r="G34" s="25" t="n">
+      <c r="G34" s="43" t="n">
         <v>3972.9123</v>
       </c>
-      <c r="H34" s="26" t="n">
+      <c r="H34" s="44" t="n">
         <v>6474.3756</v>
       </c>
     </row>
@@ -1806,10 +1824,10 @@
       <c r="F35" s="0" t="n">
         <v>1645.0</v>
       </c>
-      <c r="G35" s="25" t="n">
+      <c r="G35" s="43" t="n">
         <v>5444.3613000000005</v>
       </c>
-      <c r="H35" s="26" t="n">
+      <c r="H35" s="44" t="n">
         <v>8681.5491</v>
       </c>
     </row>
@@ -1832,10 +1850,10 @@
       <c r="F36" s="0" t="n">
         <v>1897.0</v>
       </c>
-      <c r="G36" s="25" t="n">
+      <c r="G36" s="43" t="n">
         <v>5002.926600000001</v>
       </c>
-      <c r="H36" s="26" t="n">
+      <c r="H36" s="44" t="n">
         <v>9858.7083</v>
       </c>
     </row>
@@ -1858,10 +1876,10 @@
       <c r="F37" s="0" t="n">
         <v>5841.0</v>
       </c>
-      <c r="G37" s="25" t="n">
+      <c r="G37" s="43" t="n">
         <v>7504.3899</v>
       </c>
-      <c r="H37" s="26" t="n">
+      <c r="H37" s="44" t="n">
         <v>13390.1859</v>
       </c>
     </row>
@@ -1884,10 +1902,10 @@
       <c r="F38" s="0" t="n">
         <v>737.0</v>
       </c>
-      <c r="G38" s="25" t="n">
+      <c r="G38" s="43" t="n">
         <v>6327.2307</v>
       </c>
-      <c r="H38" s="26" t="n">
+      <c r="H38" s="44" t="n">
         <v>12801.606300000001</v>
       </c>
     </row>
@@ -1910,10 +1928,10 @@
       <c r="F39" s="0" t="n">
         <v>3501.0</v>
       </c>
-      <c r="G39" s="25" t="n">
+      <c r="G39" s="43" t="n">
         <v>5885.796</v>
       </c>
-      <c r="H39" s="26" t="n">
+      <c r="H39" s="44" t="n">
         <v>13390.1859</v>
       </c>
     </row>
@@ -1936,10 +1954,10 @@
       <c r="F40" s="0" t="n">
         <v>9653.0</v>
       </c>
-      <c r="G40" s="25" t="n">
+      <c r="G40" s="43" t="n">
         <v>10152.9981</v>
       </c>
-      <c r="H40" s="26" t="n">
+      <c r="H40" s="44" t="n">
         <v>14714.490000000002</v>
       </c>
     </row>
@@ -1962,10 +1980,10 @@
       <c r="F41" s="0" t="n">
         <v>7083.0</v>
       </c>
-      <c r="G41" s="25" t="n">
+      <c r="G41" s="43" t="n">
         <v>5002.926600000001</v>
       </c>
-      <c r="H41" s="26" t="n">
+      <c r="H41" s="44" t="n">
         <v>10594.4328</v>
       </c>
     </row>
@@ -1988,10 +2006,10 @@
       <c r="F42" s="0" t="n">
         <v>6934.0</v>
       </c>
-      <c r="G42" s="25" t="n">
+      <c r="G42" s="43" t="n">
         <v>6915.8103</v>
       </c>
-      <c r="H42" s="26" t="n">
+      <c r="H42" s="44" t="n">
         <v>14861.634900000001</v>
       </c>
     </row>
@@ -2014,10 +2032,10 @@
       <c r="F43" s="0" t="n">
         <v>7106.0</v>
       </c>
-      <c r="G43" s="25" t="n">
+      <c r="G43" s="43" t="n">
         <v>8681.5491</v>
       </c>
-      <c r="H43" s="26" t="n">
+      <c r="H43" s="44" t="n">
         <v>17510.2431</v>
       </c>
     </row>
@@ -2040,10 +2058,10 @@
       <c r="F44" s="0" t="n">
         <v>551.0</v>
       </c>
-      <c r="G44" s="25" t="n">
+      <c r="G44" s="43" t="n">
         <v>7945.8246</v>
       </c>
-      <c r="H44" s="26" t="n">
+      <c r="H44" s="44" t="n">
         <v>11771.592</v>
       </c>
     </row>
@@ -2066,10 +2084,10 @@
       <c r="F45" s="0" t="n">
         <v>8820.0</v>
       </c>
-      <c r="G45" s="25" t="n">
+      <c r="G45" s="43" t="n">
         <v>5297.2164</v>
       </c>
-      <c r="H45" s="26" t="n">
+      <c r="H45" s="44" t="n">
         <v>10888.722600000001</v>
       </c>
     </row>
@@ -2092,10 +2110,10 @@
       <c r="F46" s="0" t="n">
         <v>4857.0</v>
       </c>
-      <c r="G46" s="25" t="n">
+      <c r="G46" s="43" t="n">
         <v>4855.7817000000005</v>
       </c>
-      <c r="H46" s="26" t="n">
+      <c r="H46" s="44" t="n">
         <v>7357.245000000001</v>
       </c>
     </row>
@@ -2104,7 +2122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2125,7 +2143,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B2" t="n">
         <v>1.0</v>
@@ -2136,7 +2154,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B3" t="n">
         <v>4.0</v>
@@ -2147,7 +2165,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="B4" t="n">
         <v>6.0</v>
@@ -2158,7 +2176,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="B5" t="n">
         <v>11.0</v>
@@ -2169,7 +2187,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="B6" t="n">
         <v>1.0</v>
@@ -2180,7 +2198,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="B7" t="n">
         <v>4.0</v>
@@ -2194,9 +2212,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="false"/>
   </sheetViews>
@@ -2206,9 +2224,8 @@
     <col min="2" max="2" width="19.48828125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.89453125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.65625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="11.203125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="19.42578125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="10.39453125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="19.42578125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.39453125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2225,12 +2242,9 @@
         <v>149</v>
       </c>
       <c r="E1" t="s">
-        <v>158</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2245,15 +2259,12 @@
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2300.0</v>
-      </c>
-      <c r="F2" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E2" s="45" t="n">
         <v>338433.27</v>
       </c>
-      <c r="G2" t="n">
+      <c r="F2" t="n">
         <v>23.0</v>
       </c>
     </row>
@@ -2268,15 +2279,12 @@
         <v>40</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>3400.0</v>
-      </c>
-      <c r="F3" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E3" s="45" t="n">
         <v>500292.66000000003</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="F3" s="0" t="n">
         <v>34.0</v>
       </c>
     </row>
@@ -2291,15 +2299,12 @@
         <v>59</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>3100.0</v>
-      </c>
-      <c r="F4" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E4" s="45" t="n">
         <v>456149.19</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="F4" s="0" t="n">
         <v>31.0</v>
       </c>
     </row>
@@ -2314,15 +2319,12 @@
         <v>65</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>3844.0</v>
-      </c>
-      <c r="F5" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E5" s="45" t="n">
         <v>565624.9956</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="F5" s="0" t="n">
         <v>50.0</v>
       </c>
     </row>
@@ -2337,15 +2339,12 @@
         <v>69</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>1986.8</v>
-      </c>
-      <c r="F6" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E6" s="45" t="n">
         <v>292347.48732</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="F6" s="0" t="n">
         <v>40.0</v>
       </c>
     </row>
@@ -2360,15 +2359,12 @@
         <v>92</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>2658.96</v>
-      </c>
-      <c r="F7" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E7" s="45" t="n">
         <v>391252.40330400004</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="F7" s="0" t="n">
         <v>27.0</v>
       </c>
     </row>
@@ -2383,15 +2379,12 @@
         <v>94</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>1851.0</v>
-      </c>
-      <c r="F8" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E8" s="45" t="n">
         <v>272365.2099</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="F8" s="0" t="n">
         <v>30.0</v>
       </c>
     </row>
@@ -2406,15 +2399,12 @@
         <v>107</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>2018.4</v>
-      </c>
-      <c r="F9" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E9" s="45" t="n">
         <v>296997.26616</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="F9" s="0" t="n">
         <v>29.0</v>
       </c>
     </row>
@@ -2429,15 +2419,12 @@
         <v>111</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>2840.0</v>
-      </c>
-      <c r="F10" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E10" s="45" t="n">
         <v>417891.516</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="F10" s="0" t="n">
         <v>40.0</v>
       </c>
     </row>
@@ -2452,15 +2439,12 @@
         <v>113</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>3675.86</v>
-      </c>
-      <c r="F11" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E11" s="45" t="n">
         <v>540884.0521140001</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="F11" s="0" t="n">
         <v>46.0</v>
       </c>
     </row>
@@ -2475,15 +2459,12 @@
         <v>118</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>2307.24</v>
-      </c>
-      <c r="F12" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E12" s="45" t="n">
         <v>339498.599076</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="F12" s="0" t="n">
         <v>39.0</v>
       </c>
     </row>
@@ -2498,15 +2479,12 @@
         <v>120</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>1763.86</v>
-      </c>
-      <c r="F13" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E13" s="45" t="n">
         <v>259543.003314</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="F13" s="0" t="n">
         <v>43.0</v>
       </c>
     </row>
@@ -2521,15 +2499,12 @@
         <v>128</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>1649.55</v>
-      </c>
-      <c r="F14" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E14" s="45" t="n">
         <v>242722.869795</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="F14" s="0" t="n">
         <v>21.0</v>
       </c>
     </row>
@@ -2544,15 +2519,12 @@
         <v>134</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>2592.72</v>
-      </c>
-      <c r="F15" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E15" s="45" t="n">
         <v>381505.525128</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="F15" s="0" t="n">
         <v>26.0</v>
       </c>
     </row>
@@ -2567,15 +2539,12 @@
         <v>141</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>2500.0</v>
-      </c>
-      <c r="F16" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E16" s="45" t="n">
         <v>367862.25</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="F16" s="0" t="n">
         <v>25.0</v>
       </c>
     </row>
@@ -2590,15 +2559,12 @@
         <v>143</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>2678.4</v>
-      </c>
-      <c r="F17" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E17" s="45" t="n">
         <v>394112.90016</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="F17" s="0" t="n">
         <v>31.0</v>
       </c>
     </row>
@@ -2613,15 +2579,12 @@
         <v>145</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>2953.86</v>
-      </c>
-      <c r="F18" s="27" t="n">
+        <v>166</v>
+      </c>
+      <c r="E18" s="45" t="n">
         <v>434645.434314</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="F18" s="0" t="n">
         <v>42.0</v>
       </c>
     </row>
@@ -2636,15 +2599,12 @@
         <v>57</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>4100.0</v>
-      </c>
-      <c r="F19" s="27" t="n">
+        <v>169</v>
+      </c>
+      <c r="E19" s="45" t="n">
         <v>603294.0900000001</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="F19" s="0" t="n">
         <v>41.0</v>
       </c>
     </row>
@@ -2659,15 +2619,12 @@
         <v>62</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>3700.0</v>
-      </c>
-      <c r="F20" s="27" t="n">
+        <v>169</v>
+      </c>
+      <c r="E20" s="45" t="n">
         <v>544436.13</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="F20" s="0" t="n">
         <v>37.0</v>
       </c>
     </row>
@@ -2682,15 +2639,12 @@
         <v>79</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>3700.0</v>
-      </c>
-      <c r="F21" s="27" t="n">
+        <v>169</v>
+      </c>
+      <c r="E21" s="45" t="n">
         <v>544436.13</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="F21" s="0" t="n">
         <v>37.0</v>
       </c>
     </row>
@@ -2705,15 +2659,12 @@
         <v>31</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>3200.0</v>
-      </c>
-      <c r="F22" s="27" t="n">
+        <v>171</v>
+      </c>
+      <c r="E22" s="45" t="n">
         <v>470863.68000000005</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="F22" s="0" t="n">
         <v>32.0</v>
       </c>
     </row>
@@ -2728,15 +2679,12 @@
         <v>43</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>4100.0</v>
-      </c>
-      <c r="F23" s="27" t="n">
+        <v>171</v>
+      </c>
+      <c r="E23" s="45" t="n">
         <v>603294.0900000001</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="F23" s="0" t="n">
         <v>41.0</v>
       </c>
     </row>
@@ -2751,15 +2699,12 @@
         <v>54</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>4100.0</v>
-      </c>
-      <c r="F24" s="27" t="n">
+        <v>171</v>
+      </c>
+      <c r="E24" s="45" t="n">
         <v>603294.0900000001</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="F24" s="0" t="n">
         <v>41.0</v>
       </c>
     </row>
@@ -2774,15 +2719,12 @@
         <v>86</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>1257.27</v>
-      </c>
-      <c r="F25" s="27" t="n">
+        <v>171</v>
+      </c>
+      <c r="E25" s="45" t="n">
         <v>185000.868423</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="F25" s="0" t="n">
         <v>21.0</v>
       </c>
     </row>
@@ -2797,15 +2739,12 @@
         <v>116</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>1228.2</v>
-      </c>
-      <c r="F26" s="27" t="n">
+        <v>171</v>
+      </c>
+      <c r="E26" s="45" t="n">
         <v>180723.36618</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="F26" s="0" t="n">
         <v>20.0</v>
       </c>
     </row>
@@ -2820,15 +2759,12 @@
         <v>139</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>3641.4</v>
-      </c>
-      <c r="F27" s="27" t="n">
+        <v>171</v>
+      </c>
+      <c r="E27" s="45" t="n">
         <v>535813.43886</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="F27" s="0" t="n">
         <v>45.0</v>
       </c>
     </row>
@@ -2843,15 +2779,12 @@
         <v>36</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E28" s="0" t="n">
-        <v>2756.8</v>
-      </c>
-      <c r="F28" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E28" s="45" t="n">
         <v>405649.06032000005</v>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="F28" s="0" t="n">
         <v>40.0</v>
       </c>
     </row>
@@ -2866,15 +2799,12 @@
         <v>40</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E29" s="0" t="n">
-        <v>2990.13</v>
-      </c>
-      <c r="F29" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E29" s="45" t="n">
         <v>439982.37983700004</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="F29" s="0" t="n">
         <v>39.0</v>
       </c>
     </row>
@@ -2889,15 +2819,12 @@
         <v>65</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>2700.0</v>
-      </c>
-      <c r="F30" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E30" s="45" t="n">
         <v>397291.23000000004</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="F30" s="0" t="n">
         <v>27.0</v>
       </c>
     </row>
@@ -2912,15 +2839,12 @@
         <v>69</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E31" s="0" t="n">
-        <v>1864.8</v>
-      </c>
-      <c r="F31" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E31" s="45" t="n">
         <v>274395.80952</v>
       </c>
-      <c r="G31" s="0" t="n">
+      <c r="F31" s="0" t="n">
         <v>30.0</v>
       </c>
     </row>
@@ -2935,15 +2859,12 @@
         <v>88</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E32" s="0" t="n">
-        <v>2278.53</v>
-      </c>
-      <c r="F32" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E32" s="45" t="n">
         <v>335274.06899700005</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="F32" s="0" t="n">
         <v>27.0</v>
       </c>
     </row>
@@ -2958,15 +2879,12 @@
         <v>92</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E33" s="0" t="n">
-        <v>1063.65</v>
-      </c>
-      <c r="F33" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E33" s="45" t="n">
         <v>156510.672885</v>
       </c>
-      <c r="G33" s="0" t="n">
+      <c r="F33" s="0" t="n">
         <v>21.0</v>
       </c>
     </row>
@@ -2981,15 +2899,12 @@
         <v>99</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <v>5500.0</v>
-      </c>
-      <c r="F34" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E34" s="45" t="n">
         <v>809296.9500000001</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="F34" s="0" t="n">
         <v>55.0</v>
       </c>
     </row>
@@ -3004,15 +2919,12 @@
         <v>101</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <v>5500.0</v>
-      </c>
-      <c r="F35" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E35" s="45" t="n">
         <v>809296.9500000001</v>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="F35" s="0" t="n">
         <v>55.0</v>
       </c>
     </row>
@@ -3027,15 +2939,12 @@
         <v>103</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E36" s="0" t="n">
-        <v>2891.01</v>
-      </c>
-      <c r="F36" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E36" s="45" t="n">
         <v>425397.3773490001</v>
       </c>
-      <c r="G36" s="0" t="n">
+      <c r="F36" s="0" t="n">
         <v>29.0</v>
       </c>
     </row>
@@ -3050,15 +2959,12 @@
         <v>105</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E37" s="0" t="n">
-        <v>2493.12</v>
-      </c>
-      <c r="F37" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E37" s="45" t="n">
         <v>366849.893088</v>
       </c>
-      <c r="G37" s="0" t="n">
+      <c r="F37" s="0" t="n">
         <v>42.0</v>
       </c>
     </row>
@@ -3073,15 +2979,12 @@
         <v>107</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>4361.4</v>
-      </c>
-      <c r="F38" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E38" s="45" t="n">
         <v>641757.76686</v>
       </c>
-      <c r="G38" s="0" t="n">
+      <c r="F38" s="0" t="n">
         <v>45.0</v>
       </c>
     </row>
@@ -3096,15 +2999,12 @@
         <v>125</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E39" s="0" t="n">
-        <v>2200.0</v>
-      </c>
-      <c r="F39" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E39" s="45" t="n">
         <v>323718.78</v>
       </c>
-      <c r="G39" s="0" t="n">
+      <c r="F39" s="0" t="n">
         <v>22.0</v>
       </c>
     </row>
@@ -3119,15 +3019,12 @@
         <v>132</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E40" s="0" t="n">
-        <v>3918.75</v>
-      </c>
-      <c r="F40" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E40" s="45" t="n">
         <v>576624.076875</v>
       </c>
-      <c r="G40" s="0" t="n">
+      <c r="F40" s="0" t="n">
         <v>55.0</v>
       </c>
     </row>
@@ -3142,15 +3039,12 @@
         <v>137</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E41" s="0" t="n">
-        <v>3717.5</v>
-      </c>
-      <c r="F41" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E41" s="45" t="n">
         <v>547011.16575</v>
       </c>
-      <c r="G41" s="0" t="n">
+      <c r="F41" s="0" t="n">
         <v>50.0</v>
       </c>
     </row>
@@ -3165,15 +3059,12 @@
         <v>145</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>2893.0</v>
-      </c>
-      <c r="F42" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E42" s="45" t="n">
         <v>425690.19570000004</v>
       </c>
-      <c r="G42" s="0" t="n">
+      <c r="F42" s="0" t="n">
         <v>50.0</v>
       </c>
     </row>
@@ -3188,15 +3079,12 @@
         <v>147</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E43" s="0" t="n">
-        <v>2060.37</v>
-      </c>
-      <c r="F43" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="E43" s="45" t="n">
         <v>303172.937613</v>
       </c>
-      <c r="G43" s="0" t="n">
+      <c r="F43" s="0" t="n">
         <v>27.0</v>
       </c>
     </row>
@@ -3211,15 +3099,12 @@
         <v>48</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <v>4000.0</v>
-      </c>
-      <c r="F44" s="27" t="n">
+        <v>176</v>
+      </c>
+      <c r="E44" s="45" t="n">
         <v>588579.6</v>
       </c>
-      <c r="G44" s="0" t="n">
+      <c r="F44" s="0" t="n">
         <v>40.0</v>
       </c>
     </row>
@@ -3234,15 +3119,12 @@
         <v>51</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <v>3400.0</v>
-      </c>
-      <c r="F45" s="27" t="n">
+        <v>176</v>
+      </c>
+      <c r="E45" s="45" t="n">
         <v>500292.66000000003</v>
       </c>
-      <c r="G45" s="0" t="n">
+      <c r="F45" s="0" t="n">
         <v>34.0</v>
       </c>
     </row>
@@ -3257,15 +3139,12 @@
         <v>71</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="E46" s="0" t="n">
-        <v>2800.0</v>
-      </c>
-      <c r="F46" s="27" t="n">
+        <v>176</v>
+      </c>
+      <c r="E46" s="45" t="n">
         <v>412005.72000000003</v>
       </c>
-      <c r="G46" s="0" t="n">
+      <c r="F46" s="0" t="n">
         <v>28.0</v>
       </c>
     </row>
@@ -3280,15 +3159,12 @@
         <v>75</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="E47" s="0" t="n">
-        <v>2117.75</v>
-      </c>
-      <c r="F47" s="27" t="n">
+        <v>176</v>
+      </c>
+      <c r="E47" s="45" t="n">
         <v>311616.111975</v>
       </c>
-      <c r="G47" s="0" t="n">
+      <c r="F47" s="0" t="n">
         <v>25.0</v>
       </c>
     </row>
@@ -3303,15 +3179,12 @@
         <v>81</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="E48" s="0" t="n">
-        <v>4800.0</v>
-      </c>
-      <c r="F48" s="27" t="n">
+        <v>176</v>
+      </c>
+      <c r="E48" s="45" t="n">
         <v>706295.52</v>
       </c>
-      <c r="G48" s="0" t="n">
+      <c r="F48" s="0" t="n">
         <v>48.0</v>
       </c>
     </row>
@@ -3326,15 +3199,12 @@
         <v>83</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="E49" s="0" t="n">
-        <v>3562.49</v>
-      </c>
-      <c r="F49" s="27" t="n">
+        <v>176</v>
+      </c>
+      <c r="E49" s="45" t="n">
         <v>524202.234801</v>
       </c>
-      <c r="G49" s="0" t="n">
+      <c r="F49" s="0" t="n">
         <v>41.0</v>
       </c>
     </row>
@@ -3349,15 +3219,12 @@
         <v>96</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="E50" s="0" t="n">
-        <v>3700.0</v>
-      </c>
-      <c r="F50" s="27" t="n">
+        <v>176</v>
+      </c>
+      <c r="E50" s="45" t="n">
         <v>544436.13</v>
       </c>
-      <c r="G50" s="0" t="n">
+      <c r="F50" s="0" t="n">
         <v>37.0</v>
       </c>
     </row>
@@ -3372,15 +3239,12 @@
         <v>123</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="E51" s="0" t="n">
-        <v>1405.92</v>
-      </c>
-      <c r="F51" s="27" t="n">
+        <v>176</v>
+      </c>
+      <c r="E51" s="45" t="n">
         <v>206873.957808</v>
       </c>
-      <c r="G51" s="0" t="n">
+      <c r="F51" s="0" t="n">
         <v>24.0</v>
       </c>
     </row>
@@ -3395,15 +3259,12 @@
         <v>130</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="E52" s="0" t="n">
-        <v>4400.0</v>
-      </c>
-      <c r="F52" s="27" t="n">
+        <v>176</v>
+      </c>
+      <c r="E52" s="45" t="n">
         <v>647437.56</v>
       </c>
-      <c r="G52" s="0" t="n">
+      <c r="F52" s="0" t="n">
         <v>44.0</v>
       </c>
     </row>
@@ -3418,15 +3279,12 @@
         <v>109</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="E53" s="0" t="n">
-        <v>553.95</v>
-      </c>
-      <c r="F53" s="27" t="n">
+        <v>179</v>
+      </c>
+      <c r="E53" s="45" t="n">
         <v>81510.91735500001</v>
       </c>
-      <c r="G53" s="0" t="n">
+      <c r="F53" s="0" t="n">
         <v>15.0</v>
       </c>
     </row>

</xml_diff>